<commit_message>
re-run BAADTbVT and BCDTRtSY (using updated/overwritten SYVbT)
</commit_message>
<xml_diff>
--- a/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
+++ b/InputData/trans/BCDTRtSY/BAU Cargo Dist Transported Relative to Start Yr.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="820" yWindow="460" windowWidth="17800" windowHeight="10060" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="280" windowWidth="10800" windowHeight="9920" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="About" sheetId="1" state="visible" r:id="rId1"/>
@@ -1162,11 +1162,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="173">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,78 +1419,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Rail shipments 93-97"/>
-      <sheetName val="Waterborne Flows 93-97"/>
-      <sheetName val="Air and vessel 93-97"/>
-      <sheetName val="Figure 2 compare"/>
-      <sheetName val="Factors Comparisons"/>
       <sheetName val="1997  Table 1a Modified"/>
-      <sheetName val="Figure 1"/>
-      <sheetName val="1993-97 Table 1  US Highlights"/>
-      <sheetName val="93-97 US Freight Table 1"/>
-      <sheetName val="93-97 US Freight Table 1 (b)"/>
-      <sheetName val="93-97 Percents Tab 2&amp;3"/>
-      <sheetName val="Integrated View 93-97"/>
-      <sheetName val="Figure 3 modal shares"/>
-      <sheetName val="1993-97 Percents"/>
-      <sheetName val="BTS &amp; ORNL estimates"/>
-      <sheetName val="Oil Pipeline (2)"/>
-      <sheetName val="1997 Table 2"/>
-      <sheetName val="Table 4 Distance"/>
-      <sheetName val="Distance percent change"/>
-      <sheetName val="Distance 93-97"/>
-      <sheetName val="Distance Fig value per ton"/>
-      <sheetName val="Distance Bar"/>
-      <sheetName val="Table 5 Size 93-97"/>
-      <sheetName val="Size percent change"/>
-      <sheetName val="Size Fig value per ton"/>
-      <sheetName val="Size Bar "/>
-      <sheetName val="BTS Mode"/>
-      <sheetName val="Ton-miles data"/>
-      <sheetName val="Ton-miles figure"/>
-      <sheetName val="table 3 commodities"/>
-      <sheetName val="Commodities ranked by value"/>
-      <sheetName val="Commod ranked by tons"/>
-      <sheetName val="Commod ranked by ton-miles"/>
-      <sheetName val="Commod ranked by miles per ton "/>
-      <sheetName val="Commod ranked by val per ton"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1793,10 +1725,10 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="13.33203125" customWidth="1" style="18" min="1" max="1"/>
-    <col width="107.33203125" customWidth="1" style="18" min="2" max="2"/>
+    <col width="13.36328125" customWidth="1" style="18" min="1" max="1"/>
+    <col width="107.36328125" customWidth="1" style="18" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1805,7 +1737,12 @@
           <t>BCDTRtSY BAU Cargo Dist Transported Relative to Start Year</t>
         </is>
       </c>
-      <c r="C1" s="47" t="n">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="C1" s="45" t="n">
         <v>44307</v>
       </c>
     </row>
@@ -1950,10 +1887,10 @@
       <selection activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="7.83203125" customWidth="1" style="18" min="1" max="1"/>
-    <col width="45.6640625" customWidth="1" style="18" min="2" max="2"/>
+    <col width="7.81640625" customWidth="1" style="18" min="1" max="1"/>
+    <col width="45.6328125" customWidth="1" style="18" min="2" max="2"/>
     <col width="8" customWidth="1" style="18" min="38" max="38"/>
   </cols>
   <sheetData>
@@ -8829,46 +8766,46 @@
     </row>
     <row r="86" ht="15" customHeight="1" s="18" thickBot="1"/>
     <row r="87" ht="15" customHeight="1" s="18">
-      <c r="B87" s="45" t="inlineStr">
+      <c r="B87" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Commercial trucks 8,501 to 10,000 pounds gross vehicle weight rating.</t>
         </is>
       </c>
-      <c r="C87" s="46" t="n"/>
-      <c r="D87" s="46" t="n"/>
-      <c r="E87" s="46" t="n"/>
-      <c r="F87" s="46" t="n"/>
-      <c r="G87" s="46" t="n"/>
-      <c r="H87" s="46" t="n"/>
-      <c r="I87" s="46" t="n"/>
-      <c r="J87" s="46" t="n"/>
-      <c r="K87" s="46" t="n"/>
-      <c r="L87" s="46" t="n"/>
-      <c r="M87" s="46" t="n"/>
-      <c r="N87" s="46" t="n"/>
-      <c r="O87" s="46" t="n"/>
-      <c r="P87" s="46" t="n"/>
-      <c r="Q87" s="46" t="n"/>
-      <c r="R87" s="46" t="n"/>
-      <c r="S87" s="46" t="n"/>
-      <c r="T87" s="46" t="n"/>
-      <c r="U87" s="46" t="n"/>
-      <c r="V87" s="46" t="n"/>
-      <c r="W87" s="46" t="n"/>
-      <c r="X87" s="46" t="n"/>
-      <c r="Y87" s="46" t="n"/>
-      <c r="Z87" s="46" t="n"/>
-      <c r="AA87" s="46" t="n"/>
-      <c r="AB87" s="46" t="n"/>
-      <c r="AC87" s="46" t="n"/>
-      <c r="AD87" s="46" t="n"/>
-      <c r="AE87" s="46" t="n"/>
-      <c r="AF87" s="46" t="n"/>
-      <c r="AG87" s="46" t="n"/>
-      <c r="AH87" s="46" t="n"/>
-      <c r="AI87" s="46" t="n"/>
-      <c r="AJ87" s="46" t="n"/>
-      <c r="AK87" s="46" t="n"/>
+      <c r="C87" s="47" t="n"/>
+      <c r="D87" s="47" t="n"/>
+      <c r="E87" s="47" t="n"/>
+      <c r="F87" s="47" t="n"/>
+      <c r="G87" s="47" t="n"/>
+      <c r="H87" s="47" t="n"/>
+      <c r="I87" s="47" t="n"/>
+      <c r="J87" s="47" t="n"/>
+      <c r="K87" s="47" t="n"/>
+      <c r="L87" s="47" t="n"/>
+      <c r="M87" s="47" t="n"/>
+      <c r="N87" s="47" t="n"/>
+      <c r="O87" s="47" t="n"/>
+      <c r="P87" s="47" t="n"/>
+      <c r="Q87" s="47" t="n"/>
+      <c r="R87" s="47" t="n"/>
+      <c r="S87" s="47" t="n"/>
+      <c r="T87" s="47" t="n"/>
+      <c r="U87" s="47" t="n"/>
+      <c r="V87" s="47" t="n"/>
+      <c r="W87" s="47" t="n"/>
+      <c r="X87" s="47" t="n"/>
+      <c r="Y87" s="47" t="n"/>
+      <c r="Z87" s="47" t="n"/>
+      <c r="AA87" s="47" t="n"/>
+      <c r="AB87" s="47" t="n"/>
+      <c r="AC87" s="47" t="n"/>
+      <c r="AD87" s="47" t="n"/>
+      <c r="AE87" s="47" t="n"/>
+      <c r="AF87" s="47" t="n"/>
+      <c r="AG87" s="47" t="n"/>
+      <c r="AH87" s="47" t="n"/>
+      <c r="AI87" s="47" t="n"/>
+      <c r="AJ87" s="47" t="n"/>
+      <c r="AK87" s="47" t="n"/>
     </row>
     <row r="88" ht="15" customHeight="1" s="18">
       <c r="B88" s="7" t="inlineStr">
@@ -9030,7 +8967,7 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" ht="14.75" customHeight="1" s="18" thickBot="1">
       <c r="A1" s="29" t="n"/>
@@ -10602,7 +10539,7 @@
         <v>-0.002863</v>
       </c>
     </row>
-    <row r="24" ht="27" customHeight="1" s="18">
+    <row r="24" ht="24.5" customHeight="1" s="18">
       <c r="A24" s="32" t="inlineStr">
         <is>
           <t>TEU000:ba_Intercity</t>
@@ -11966,7 +11903,7 @@
         <v>-0.005808</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" ht="24.5" customHeight="1" s="18">
       <c r="A37" s="32" t="inlineStr">
         <is>
           <t>TEU000:ca_Water</t>
@@ -16014,47 +15951,47 @@
     </row>
     <row r="76">
       <c r="A76" s="29" t="n"/>
-      <c r="B76" s="45" t="inlineStr">
+      <c r="B76" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Commercial light trucks from 8,501 to 10,000 pounds.</t>
         </is>
       </c>
-      <c r="C76" s="46" t="n"/>
-      <c r="D76" s="46" t="n"/>
-      <c r="E76" s="46" t="n"/>
-      <c r="F76" s="46" t="n"/>
-      <c r="G76" s="46" t="n"/>
-      <c r="H76" s="46" t="n"/>
-      <c r="I76" s="46" t="n"/>
-      <c r="J76" s="46" t="n"/>
-      <c r="K76" s="46" t="n"/>
-      <c r="L76" s="46" t="n"/>
-      <c r="M76" s="46" t="n"/>
-      <c r="N76" s="46" t="n"/>
-      <c r="O76" s="46" t="n"/>
-      <c r="P76" s="46" t="n"/>
-      <c r="Q76" s="46" t="n"/>
-      <c r="R76" s="46" t="n"/>
-      <c r="S76" s="46" t="n"/>
-      <c r="T76" s="46" t="n"/>
-      <c r="U76" s="46" t="n"/>
-      <c r="V76" s="46" t="n"/>
-      <c r="W76" s="46" t="n"/>
-      <c r="X76" s="46" t="n"/>
-      <c r="Y76" s="46" t="n"/>
-      <c r="Z76" s="46" t="n"/>
-      <c r="AA76" s="46" t="n"/>
-      <c r="AB76" s="46" t="n"/>
-      <c r="AC76" s="46" t="n"/>
-      <c r="AD76" s="46" t="n"/>
-      <c r="AE76" s="46" t="n"/>
-      <c r="AF76" s="46" t="n"/>
-      <c r="AG76" s="46" t="n"/>
-      <c r="AH76" s="46" t="n"/>
-      <c r="AI76" s="46" t="n"/>
-      <c r="AJ76" s="46" t="n"/>
-      <c r="AK76" s="46" t="n"/>
-      <c r="AL76" s="46" t="n"/>
+      <c r="C76" s="47" t="n"/>
+      <c r="D76" s="47" t="n"/>
+      <c r="E76" s="47" t="n"/>
+      <c r="F76" s="47" t="n"/>
+      <c r="G76" s="47" t="n"/>
+      <c r="H76" s="47" t="n"/>
+      <c r="I76" s="47" t="n"/>
+      <c r="J76" s="47" t="n"/>
+      <c r="K76" s="47" t="n"/>
+      <c r="L76" s="47" t="n"/>
+      <c r="M76" s="47" t="n"/>
+      <c r="N76" s="47" t="n"/>
+      <c r="O76" s="47" t="n"/>
+      <c r="P76" s="47" t="n"/>
+      <c r="Q76" s="47" t="n"/>
+      <c r="R76" s="47" t="n"/>
+      <c r="S76" s="47" t="n"/>
+      <c r="T76" s="47" t="n"/>
+      <c r="U76" s="47" t="n"/>
+      <c r="V76" s="47" t="n"/>
+      <c r="W76" s="47" t="n"/>
+      <c r="X76" s="47" t="n"/>
+      <c r="Y76" s="47" t="n"/>
+      <c r="Z76" s="47" t="n"/>
+      <c r="AA76" s="47" t="n"/>
+      <c r="AB76" s="47" t="n"/>
+      <c r="AC76" s="47" t="n"/>
+      <c r="AD76" s="47" t="n"/>
+      <c r="AE76" s="47" t="n"/>
+      <c r="AF76" s="47" t="n"/>
+      <c r="AG76" s="47" t="n"/>
+      <c r="AH76" s="47" t="n"/>
+      <c r="AI76" s="47" t="n"/>
+      <c r="AJ76" s="47" t="n"/>
+      <c r="AK76" s="47" t="n"/>
+      <c r="AL76" s="47" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="29" t="n"/>
@@ -16329,10 +16266,10 @@
       <selection activeCell="B59" activeCellId="1" sqref="A45:XFD45 A59:XFD59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col hidden="1" width="20.83203125" customWidth="1" style="18" min="1" max="1"/>
-    <col width="45.6640625" customWidth="1" style="18" min="2" max="2"/>
+    <col hidden="1" width="20.81640625" customWidth="1" style="18" min="1" max="1"/>
+    <col width="45.6328125" customWidth="1" style="18" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="18" thickBot="1">
@@ -35765,46 +35702,46 @@
     </row>
     <row r="204" ht="15" customHeight="1" s="18" thickBot="1"/>
     <row r="205" ht="15" customHeight="1" s="18">
-      <c r="B205" s="45" t="inlineStr">
+      <c r="B205" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Assumed to be the same as International U.S..</t>
         </is>
       </c>
-      <c r="C205" s="46" t="n"/>
-      <c r="D205" s="46" t="n"/>
-      <c r="E205" s="46" t="n"/>
-      <c r="F205" s="46" t="n"/>
-      <c r="G205" s="46" t="n"/>
-      <c r="H205" s="46" t="n"/>
-      <c r="I205" s="46" t="n"/>
-      <c r="J205" s="46" t="n"/>
-      <c r="K205" s="46" t="n"/>
-      <c r="L205" s="46" t="n"/>
-      <c r="M205" s="46" t="n"/>
-      <c r="N205" s="46" t="n"/>
-      <c r="O205" s="46" t="n"/>
-      <c r="P205" s="46" t="n"/>
-      <c r="Q205" s="46" t="n"/>
-      <c r="R205" s="46" t="n"/>
-      <c r="S205" s="46" t="n"/>
-      <c r="T205" s="46" t="n"/>
-      <c r="U205" s="46" t="n"/>
-      <c r="V205" s="46" t="n"/>
-      <c r="W205" s="46" t="n"/>
-      <c r="X205" s="46" t="n"/>
-      <c r="Y205" s="46" t="n"/>
-      <c r="Z205" s="46" t="n"/>
-      <c r="AA205" s="46" t="n"/>
-      <c r="AB205" s="46" t="n"/>
-      <c r="AC205" s="46" t="n"/>
-      <c r="AD205" s="46" t="n"/>
-      <c r="AE205" s="46" t="n"/>
-      <c r="AF205" s="46" t="n"/>
-      <c r="AG205" s="46" t="n"/>
-      <c r="AH205" s="46" t="n"/>
-      <c r="AI205" s="46" t="n"/>
-      <c r="AJ205" s="46" t="n"/>
-      <c r="AK205" s="46" t="n"/>
+      <c r="C205" s="47" t="n"/>
+      <c r="D205" s="47" t="n"/>
+      <c r="E205" s="47" t="n"/>
+      <c r="F205" s="47" t="n"/>
+      <c r="G205" s="47" t="n"/>
+      <c r="H205" s="47" t="n"/>
+      <c r="I205" s="47" t="n"/>
+      <c r="J205" s="47" t="n"/>
+      <c r="K205" s="47" t="n"/>
+      <c r="L205" s="47" t="n"/>
+      <c r="M205" s="47" t="n"/>
+      <c r="N205" s="47" t="n"/>
+      <c r="O205" s="47" t="n"/>
+      <c r="P205" s="47" t="n"/>
+      <c r="Q205" s="47" t="n"/>
+      <c r="R205" s="47" t="n"/>
+      <c r="S205" s="47" t="n"/>
+      <c r="T205" s="47" t="n"/>
+      <c r="U205" s="47" t="n"/>
+      <c r="V205" s="47" t="n"/>
+      <c r="W205" s="47" t="n"/>
+      <c r="X205" s="47" t="n"/>
+      <c r="Y205" s="47" t="n"/>
+      <c r="Z205" s="47" t="n"/>
+      <c r="AA205" s="47" t="n"/>
+      <c r="AB205" s="47" t="n"/>
+      <c r="AC205" s="47" t="n"/>
+      <c r="AD205" s="47" t="n"/>
+      <c r="AE205" s="47" t="n"/>
+      <c r="AF205" s="47" t="n"/>
+      <c r="AG205" s="47" t="n"/>
+      <c r="AH205" s="47" t="n"/>
+      <c r="AI205" s="47" t="n"/>
+      <c r="AJ205" s="47" t="n"/>
+      <c r="AK205" s="47" t="n"/>
     </row>
     <row r="206" ht="15" customHeight="1" s="18">
       <c r="B206" s="7" t="inlineStr">
@@ -35889,10 +35826,10 @@
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="10.83203125" customWidth="1" style="18" min="1" max="1"/>
-    <col width="45.6640625" customWidth="1" style="18" min="2" max="2"/>
+    <col width="10.81640625" customWidth="1" style="18" min="1" max="1"/>
+    <col width="45.6328125" customWidth="1" style="18" min="2" max="2"/>
     <col width="8" customWidth="1" style="18" min="38" max="38"/>
   </cols>
   <sheetData>
@@ -43281,46 +43218,46 @@
     </row>
     <row r="87" ht="15" customHeight="1" s="18">
       <c r="A87" s="29" t="n"/>
-      <c r="B87" s="45" t="inlineStr">
+      <c r="B87" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Commercial trucks 8,501 to 10,000 pounds gross vehicle weight rating.</t>
         </is>
       </c>
-      <c r="C87" s="46" t="n"/>
-      <c r="D87" s="46" t="n"/>
-      <c r="E87" s="46" t="n"/>
-      <c r="F87" s="46" t="n"/>
-      <c r="G87" s="46" t="n"/>
-      <c r="H87" s="46" t="n"/>
-      <c r="I87" s="46" t="n"/>
-      <c r="J87" s="46" t="n"/>
-      <c r="K87" s="46" t="n"/>
-      <c r="L87" s="46" t="n"/>
-      <c r="M87" s="46" t="n"/>
-      <c r="N87" s="46" t="n"/>
-      <c r="O87" s="46" t="n"/>
-      <c r="P87" s="46" t="n"/>
-      <c r="Q87" s="46" t="n"/>
-      <c r="R87" s="46" t="n"/>
-      <c r="S87" s="46" t="n"/>
-      <c r="T87" s="46" t="n"/>
-      <c r="U87" s="46" t="n"/>
-      <c r="V87" s="46" t="n"/>
-      <c r="W87" s="46" t="n"/>
-      <c r="X87" s="46" t="n"/>
-      <c r="Y87" s="46" t="n"/>
-      <c r="Z87" s="46" t="n"/>
-      <c r="AA87" s="46" t="n"/>
-      <c r="AB87" s="46" t="n"/>
-      <c r="AC87" s="46" t="n"/>
-      <c r="AD87" s="46" t="n"/>
-      <c r="AE87" s="46" t="n"/>
-      <c r="AF87" s="46" t="n"/>
-      <c r="AG87" s="46" t="n"/>
-      <c r="AH87" s="46" t="n"/>
-      <c r="AI87" s="46" t="n"/>
-      <c r="AJ87" s="45" t="n"/>
-      <c r="AK87" s="45" t="n"/>
+      <c r="C87" s="47" t="n"/>
+      <c r="D87" s="47" t="n"/>
+      <c r="E87" s="47" t="n"/>
+      <c r="F87" s="47" t="n"/>
+      <c r="G87" s="47" t="n"/>
+      <c r="H87" s="47" t="n"/>
+      <c r="I87" s="47" t="n"/>
+      <c r="J87" s="47" t="n"/>
+      <c r="K87" s="47" t="n"/>
+      <c r="L87" s="47" t="n"/>
+      <c r="M87" s="47" t="n"/>
+      <c r="N87" s="47" t="n"/>
+      <c r="O87" s="47" t="n"/>
+      <c r="P87" s="47" t="n"/>
+      <c r="Q87" s="47" t="n"/>
+      <c r="R87" s="47" t="n"/>
+      <c r="S87" s="47" t="n"/>
+      <c r="T87" s="47" t="n"/>
+      <c r="U87" s="47" t="n"/>
+      <c r="V87" s="47" t="n"/>
+      <c r="W87" s="47" t="n"/>
+      <c r="X87" s="47" t="n"/>
+      <c r="Y87" s="47" t="n"/>
+      <c r="Z87" s="47" t="n"/>
+      <c r="AA87" s="47" t="n"/>
+      <c r="AB87" s="47" t="n"/>
+      <c r="AC87" s="47" t="n"/>
+      <c r="AD87" s="47" t="n"/>
+      <c r="AE87" s="47" t="n"/>
+      <c r="AF87" s="47" t="n"/>
+      <c r="AG87" s="47" t="n"/>
+      <c r="AH87" s="47" t="n"/>
+      <c r="AI87" s="47" t="n"/>
+      <c r="AJ87" s="46" t="n"/>
+      <c r="AK87" s="46" t="n"/>
     </row>
     <row r="88" ht="15" customHeight="1" s="18">
       <c r="A88" s="29" t="n"/>
@@ -43746,9 +43683,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="15.83203125" customWidth="1" style="18" min="1" max="1"/>
+    <col width="15.81640625" customWidth="1" style="18" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.75" customHeight="1" s="18" thickBot="1">
@@ -45216,7 +45153,7 @@
       </c>
       <c r="AJ23" s="1" t="n"/>
     </row>
-    <row r="24" ht="27" customHeight="1" s="18">
+    <row r="24" ht="24.5" customHeight="1" s="18">
       <c r="A24" s="32" t="inlineStr">
         <is>
           <t>TEU000:ba_Intercity</t>
@@ -46489,7 +46426,7 @@
       </c>
       <c r="AJ36" s="1" t="n"/>
     </row>
-    <row r="37">
+    <row r="37" ht="24.5" customHeight="1" s="18">
       <c r="A37" s="32" t="inlineStr">
         <is>
           <t>TEU000:ca_Water</t>
@@ -50267,45 +50204,45 @@
     </row>
     <row r="76">
       <c r="A76" s="29" t="n"/>
-      <c r="B76" s="45" t="inlineStr">
+      <c r="B76" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Commercial light trucks from 8,501 to 10,000 pounds.</t>
         </is>
       </c>
-      <c r="C76" s="46" t="n"/>
-      <c r="D76" s="46" t="n"/>
-      <c r="E76" s="46" t="n"/>
-      <c r="F76" s="46" t="n"/>
-      <c r="G76" s="46" t="n"/>
-      <c r="H76" s="46" t="n"/>
-      <c r="I76" s="46" t="n"/>
-      <c r="J76" s="46" t="n"/>
-      <c r="K76" s="46" t="n"/>
-      <c r="L76" s="46" t="n"/>
-      <c r="M76" s="46" t="n"/>
-      <c r="N76" s="46" t="n"/>
-      <c r="O76" s="46" t="n"/>
-      <c r="P76" s="46" t="n"/>
-      <c r="Q76" s="46" t="n"/>
-      <c r="R76" s="46" t="n"/>
-      <c r="S76" s="46" t="n"/>
-      <c r="T76" s="46" t="n"/>
-      <c r="U76" s="46" t="n"/>
-      <c r="V76" s="46" t="n"/>
-      <c r="W76" s="46" t="n"/>
-      <c r="X76" s="46" t="n"/>
-      <c r="Y76" s="46" t="n"/>
-      <c r="Z76" s="46" t="n"/>
-      <c r="AA76" s="46" t="n"/>
-      <c r="AB76" s="46" t="n"/>
-      <c r="AC76" s="46" t="n"/>
-      <c r="AD76" s="46" t="n"/>
-      <c r="AE76" s="46" t="n"/>
-      <c r="AF76" s="46" t="n"/>
-      <c r="AG76" s="46" t="n"/>
-      <c r="AH76" s="46" t="n"/>
-      <c r="AI76" s="46" t="n"/>
-      <c r="AJ76" s="45" t="n"/>
+      <c r="C76" s="47" t="n"/>
+      <c r="D76" s="47" t="n"/>
+      <c r="E76" s="47" t="n"/>
+      <c r="F76" s="47" t="n"/>
+      <c r="G76" s="47" t="n"/>
+      <c r="H76" s="47" t="n"/>
+      <c r="I76" s="47" t="n"/>
+      <c r="J76" s="47" t="n"/>
+      <c r="K76" s="47" t="n"/>
+      <c r="L76" s="47" t="n"/>
+      <c r="M76" s="47" t="n"/>
+      <c r="N76" s="47" t="n"/>
+      <c r="O76" s="47" t="n"/>
+      <c r="P76" s="47" t="n"/>
+      <c r="Q76" s="47" t="n"/>
+      <c r="R76" s="47" t="n"/>
+      <c r="S76" s="47" t="n"/>
+      <c r="T76" s="47" t="n"/>
+      <c r="U76" s="47" t="n"/>
+      <c r="V76" s="47" t="n"/>
+      <c r="W76" s="47" t="n"/>
+      <c r="X76" s="47" t="n"/>
+      <c r="Y76" s="47" t="n"/>
+      <c r="Z76" s="47" t="n"/>
+      <c r="AA76" s="47" t="n"/>
+      <c r="AB76" s="47" t="n"/>
+      <c r="AC76" s="47" t="n"/>
+      <c r="AD76" s="47" t="n"/>
+      <c r="AE76" s="47" t="n"/>
+      <c r="AF76" s="47" t="n"/>
+      <c r="AG76" s="47" t="n"/>
+      <c r="AH76" s="47" t="n"/>
+      <c r="AI76" s="47" t="n"/>
+      <c r="AJ76" s="46" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="29" t="n"/>
@@ -50549,10 +50486,10 @@
       <selection activeCell="A74" sqref="A74:XFD74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="17.6640625" customWidth="1" style="18" min="1" max="1"/>
-    <col width="45.6640625" customWidth="1" style="18" min="2" max="2"/>
+    <col width="17.6328125" customWidth="1" style="18" min="1" max="1"/>
+    <col width="45.6328125" customWidth="1" style="18" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="18" thickBot="1">
@@ -70205,46 +70142,46 @@
     </row>
     <row r="205" ht="15" customHeight="1" s="18">
       <c r="A205" s="29" t="n"/>
-      <c r="B205" s="45" t="inlineStr">
+      <c r="B205" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve">   1/ Assumed to be the same as International U.S..</t>
         </is>
       </c>
-      <c r="C205" s="46" t="n"/>
-      <c r="D205" s="46" t="n"/>
-      <c r="E205" s="46" t="n"/>
-      <c r="F205" s="46" t="n"/>
-      <c r="G205" s="46" t="n"/>
-      <c r="H205" s="46" t="n"/>
-      <c r="I205" s="46" t="n"/>
-      <c r="J205" s="46" t="n"/>
-      <c r="K205" s="46" t="n"/>
-      <c r="L205" s="46" t="n"/>
-      <c r="M205" s="46" t="n"/>
-      <c r="N205" s="46" t="n"/>
-      <c r="O205" s="46" t="n"/>
-      <c r="P205" s="46" t="n"/>
-      <c r="Q205" s="46" t="n"/>
-      <c r="R205" s="46" t="n"/>
-      <c r="S205" s="46" t="n"/>
-      <c r="T205" s="46" t="n"/>
-      <c r="U205" s="46" t="n"/>
-      <c r="V205" s="46" t="n"/>
-      <c r="W205" s="46" t="n"/>
-      <c r="X205" s="46" t="n"/>
-      <c r="Y205" s="46" t="n"/>
-      <c r="Z205" s="46" t="n"/>
-      <c r="AA205" s="46" t="n"/>
-      <c r="AB205" s="46" t="n"/>
-      <c r="AC205" s="46" t="n"/>
-      <c r="AD205" s="46" t="n"/>
-      <c r="AE205" s="46" t="n"/>
-      <c r="AF205" s="46" t="n"/>
-      <c r="AG205" s="46" t="n"/>
-      <c r="AH205" s="46" t="n"/>
-      <c r="AI205" s="46" t="n"/>
-      <c r="AJ205" s="45" t="n"/>
-      <c r="AK205" s="45" t="n"/>
+      <c r="C205" s="47" t="n"/>
+      <c r="D205" s="47" t="n"/>
+      <c r="E205" s="47" t="n"/>
+      <c r="F205" s="47" t="n"/>
+      <c r="G205" s="47" t="n"/>
+      <c r="H205" s="47" t="n"/>
+      <c r="I205" s="47" t="n"/>
+      <c r="J205" s="47" t="n"/>
+      <c r="K205" s="47" t="n"/>
+      <c r="L205" s="47" t="n"/>
+      <c r="M205" s="47" t="n"/>
+      <c r="N205" s="47" t="n"/>
+      <c r="O205" s="47" t="n"/>
+      <c r="P205" s="47" t="n"/>
+      <c r="Q205" s="47" t="n"/>
+      <c r="R205" s="47" t="n"/>
+      <c r="S205" s="47" t="n"/>
+      <c r="T205" s="47" t="n"/>
+      <c r="U205" s="47" t="n"/>
+      <c r="V205" s="47" t="n"/>
+      <c r="W205" s="47" t="n"/>
+      <c r="X205" s="47" t="n"/>
+      <c r="Y205" s="47" t="n"/>
+      <c r="Z205" s="47" t="n"/>
+      <c r="AA205" s="47" t="n"/>
+      <c r="AB205" s="47" t="n"/>
+      <c r="AC205" s="47" t="n"/>
+      <c r="AD205" s="47" t="n"/>
+      <c r="AE205" s="47" t="n"/>
+      <c r="AF205" s="47" t="n"/>
+      <c r="AG205" s="47" t="n"/>
+      <c r="AH205" s="47" t="n"/>
+      <c r="AI205" s="47" t="n"/>
+      <c r="AJ205" s="46" t="n"/>
+      <c r="AK205" s="46" t="n"/>
     </row>
     <row r="206" ht="15" customHeight="1" s="18">
       <c r="A206" s="29" t="n"/>
@@ -70421,9 +70358,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="16.6640625" customWidth="1" style="18" min="1" max="1"/>
+    <col width="16.6328125" customWidth="1" style="18" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="71.25" customHeight="1" s="18">
@@ -71264,9 +71201,9 @@
       <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="16.6640625" customWidth="1" style="18" min="1" max="1"/>
+    <col width="16.6328125" customWidth="1" style="18" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="71.25" customHeight="1" s="18">

</xml_diff>